<commit_message>
fish asemblage Abrolhos and species GAMS PT Cloates
</commit_message>
<xml_diff>
--- a/outputs/PtCloates/PtCloatesBRUVS_fishlist_GC.xlsx
+++ b/outputs/PtCloates/PtCloatesBRUVS_fishlist_GC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10522231\MEG\GC_Chapter3_BRUVSvsDropCam\outputs\PtCloates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D77800C-5431-49C7-8661-1EC8B5007C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9282C3D5-1D9E-479D-B41A-F9AA52999DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-2268" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PtCloatesBRUVS_fishlist" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,11 @@
     <sheet name="minus_Unknown_Genus" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="254">
   <si>
     <t>family</t>
   </si>
@@ -745,9 +744,6 @@
     <t>Average dumerili and rivoliana</t>
   </si>
   <si>
-    <t>asked Bri</t>
-  </si>
-  <si>
     <t>leave as spp</t>
   </si>
   <si>
@@ -761,6 +757,33 @@
   </si>
   <si>
     <t>change to Ostorhinchus semilineatus</t>
+  </si>
+  <si>
+    <t>should be sp1</t>
+  </si>
+  <si>
+    <t>keep as multidens</t>
+  </si>
+  <si>
+    <t>sp1?</t>
+  </si>
+  <si>
+    <t>YES sp1</t>
+  </si>
+  <si>
+    <t>too far away to tell, leave as spp.</t>
+  </si>
+  <si>
+    <t>no change</t>
+  </si>
+  <si>
+    <t>YES - CONFIRM W C</t>
+  </si>
+  <si>
+    <t>average filamentosus and typus</t>
+  </si>
+  <si>
+    <t>no change.</t>
   </si>
 </sst>
 </file>
@@ -6572,7 +6595,7 @@
   <dimension ref="A1:M135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6580,6 +6603,8 @@
     <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
@@ -6693,10 +6718,10 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
+        <v>243</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
@@ -7792,7 +7817,12 @@
       <c r="E68">
         <v>32</v>
       </c>
-      <c r="G68" s="1"/>
+      <c r="G68" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="I68" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
@@ -7804,17 +7834,17 @@
       <c r="C69" t="s">
         <v>121</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="1">
         <v>5</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="1">
         <v>16</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="I69" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="M69" t="s">
         <v>121</v>
@@ -7830,13 +7860,19 @@
       <c r="C70" t="s">
         <v>46</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="1">
         <v>48</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="1">
         <v>220</v>
       </c>
       <c r="G70" s="1"/>
+      <c r="K70" t="s">
+        <v>250</v>
+      </c>
+      <c r="M70" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -7854,8 +7890,14 @@
       <c r="E71">
         <v>2</v>
       </c>
-      <c r="G71" s="2" t="s">
-        <v>240</v>
+      <c r="G71" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="I71" t="s">
+        <v>249</v>
+      </c>
+      <c r="K71" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.35">
@@ -7874,7 +7916,12 @@
       <c r="E72">
         <v>1</v>
       </c>
-      <c r="G72" s="1"/>
+      <c r="G72" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="I72" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
@@ -8012,7 +8059,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>132</v>
       </c>
@@ -8029,7 +8076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>132</v>
       </c>
@@ -8046,7 +8093,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>142</v>
       </c>
@@ -8063,7 +8110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>142</v>
       </c>
@@ -8080,7 +8127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>142</v>
       </c>
@@ -8097,7 +8144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>142</v>
       </c>
@@ -8116,8 +8163,11 @@
       <c r="G86" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I86" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>147</v>
       </c>
@@ -8134,7 +8184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>147</v>
       </c>
@@ -8151,7 +8201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>147</v>
       </c>
@@ -8168,7 +8218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>147</v>
       </c>
@@ -8185,7 +8235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>147</v>
       </c>
@@ -8202,7 +8252,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>147</v>
       </c>
@@ -8219,7 +8269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>147</v>
       </c>
@@ -8236,7 +8286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>156</v>
       </c>
@@ -8253,7 +8303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>156</v>
       </c>
@@ -8270,7 +8320,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>156</v>
       </c>
@@ -8287,7 +8337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>160</v>
       </c>
@@ -8304,7 +8354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>160</v>
       </c>
@@ -8321,7 +8371,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>160</v>
       </c>
@@ -8338,7 +8388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>160</v>
       </c>
@@ -8355,7 +8405,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>168</v>
       </c>
@@ -8372,7 +8422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>171</v>
       </c>
@@ -8389,7 +8439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>174</v>
       </c>
@@ -8406,7 +8456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>179</v>
       </c>
@@ -8423,7 +8473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>179</v>
       </c>
@@ -8440,7 +8490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>183</v>
       </c>
@@ -8457,7 +8507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>183</v>
       </c>
@@ -8474,10 +8524,13 @@
         <v>13</v>
       </c>
       <c r="G107" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+        <v>240</v>
+      </c>
+      <c r="I107" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>186</v>
       </c>
@@ -8494,7 +8547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>186</v>
       </c>
@@ -8511,7 +8564,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>186</v>
       </c>
@@ -8528,7 +8581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>186</v>
       </c>
@@ -8545,7 +8598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>186</v>
       </c>
@@ -8647,10 +8700,10 @@
         <v>14</v>
       </c>
       <c r="G117" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="M117" t="s">
         <v>242</v>
-      </c>
-      <c r="M117" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.35">
@@ -8807,7 +8860,10 @@
         <v>3</v>
       </c>
       <c r="G126" t="s">
-        <v>241</v>
+        <v>240</v>
+      </c>
+      <c r="I126" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>